<commit_message>
Added new changes to Monthly Rapport and consolidated CSVs
</commit_message>
<xml_diff>
--- a/(ITA) Aug Inbound from Production.xlsx
+++ b/(ITA) Aug Inbound from Production.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\OneDrive\Documents\House of Analytics\ITA\-Ita-Data_Cleanup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{519E3FB9-DB7F-46FC-BE3F-912A57007974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B5086A-EAF8-42F0-82EF-84F14471BE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{205C0F19-93A7-4741-A05B-5E955084DEED}"/>
   </bookViews>
@@ -297,17 +297,18 @@
     <sheetNames>
       <sheetName val="Juli ref"/>
       <sheetName val="Aug25 Rapport"/>
+      <sheetName val="Stockcount Pivot"/>
       <sheetName val="Aug25 DK SHIPMENTS"/>
       <sheetName val="Aug25 DE SHIPMENTS"/>
       <sheetName val="Aug25 Ingående ordrelinje"/>
       <sheetName val="Prod Order"/>
       <sheetName val="Aug25 Prod Order-DK"/>
       <sheetName val="Aug25 Prod Order - DE"/>
-      <sheetName val="Inbound from Production"/>
       <sheetName val="Aug25 indgående fr production"/>
+      <sheetName val="Sheet5"/>
       <sheetName val="31.08.25 stockcount Skanderborg"/>
+      <sheetName val="31.08.25 stock count Flensborg"/>
       <sheetName val="31.08.25 stock count Handewitt"/>
-      <sheetName val="31.08.25 stock count Flensborg"/>
       <sheetName val="Reference_Lagerid_Country"/>
     </sheetNames>
     <sheetDataSet>
@@ -324,7 +325,8 @@
       <sheetData sheetId="10"/>
       <sheetData sheetId="11"/>
       <sheetData sheetId="12"/>
-      <sheetData sheetId="13">
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14">
         <row r="1">
           <cell r="A1" t="str">
             <v>Lagerid</v>
@@ -655,10 +657,13 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M27"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">

</xml_diff>